<commit_message>
added usage comment to ExcelWrited, deleted test page
</commit_message>
<xml_diff>
--- a/DrugProNET/Temp/spreadsheet.xlsx
+++ b/DrugProNET/Temp/spreadsheet.xlsx
@@ -81,7 +81,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -109,1682 +109,1430 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>749413.899494994</v>
+        <v>511922.456562483</v>
       </c>
       <c r="B2" s="0">
-        <v>104096.823420421</v>
+        <v>251119.751600139</v>
       </c>
       <c r="C2" s="0">
-        <v>398573.545458994</v>
+        <v>745481.11192206</v>
       </c>
       <c r="D2" s="0">
-        <v>523118.26521676</v>
+        <v>692637.938862964</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>148219.427162884</v>
+        <v>284464.639744006</v>
       </c>
       <c r="B3" s="0">
-        <v>226576.241304435</v>
+        <v>212584.139878202</v>
       </c>
       <c r="C3" s="0">
-        <v>295576.775118512</v>
+        <v>106833.798860588</v>
       </c>
       <c r="D3" s="0">
-        <v>394385.909845301</v>
+        <v>881508.007124769</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>505213.356812118</v>
+        <v>424864.378955618</v>
       </c>
       <c r="B4" s="0">
-        <v>970812.594038813</v>
+        <v>825658.15831798</v>
       </c>
       <c r="C4" s="0">
-        <v>70803.7526676449</v>
+        <v>375435.556459909</v>
       </c>
       <c r="D4" s="0">
-        <v>410644.041565547</v>
+        <v>915094.362532298</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>431656.153142292</v>
+        <v>720311.327707167</v>
       </c>
       <c r="B5" s="0">
-        <v>565299.232287937</v>
+        <v>459193.282508847</v>
       </c>
       <c r="C5" s="0">
-        <v>899672.99387775</v>
+        <v>43197.4753938604</v>
       </c>
       <c r="D5" s="0">
-        <v>323827.13692441</v>
+        <v>183529.805011828</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>494827.068641236</v>
+        <v>736430.415760926</v>
       </c>
       <c r="B6" s="0">
-        <v>273656.433109965</v>
+        <v>436458.393668969</v>
       </c>
       <c r="C6" s="0">
-        <v>915136.557964206</v>
+        <v>980171.929104334</v>
       </c>
       <c r="D6" s="0">
-        <v>928713.249475096</v>
+        <v>437503.349239707</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>916725.039909</v>
+        <v>463193.035900217</v>
       </c>
       <c r="B7" s="0">
-        <v>446754.886045472</v>
+        <v>906562.25844592</v>
       </c>
       <c r="C7" s="0">
-        <v>38635.1882659994</v>
+        <v>261415.937571514</v>
       </c>
       <c r="D7" s="0">
-        <v>288194.120995791</v>
+        <v>600484.636891859</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>944534.051671873</v>
+        <v>746328.553066742</v>
       </c>
       <c r="B8" s="0">
-        <v>676279.582398142</v>
+        <v>263596.764422765</v>
       </c>
       <c r="C8" s="0">
-        <v>353052.865878238</v>
+        <v>221804.746529928</v>
       </c>
       <c r="D8" s="0">
-        <v>410966.38627861</v>
+        <v>172177.26175309</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>578831.815896012</v>
+        <v>112452.179245861</v>
       </c>
       <c r="B9" s="0">
-        <v>251202.497282625</v>
+        <v>758714.171479789</v>
       </c>
       <c r="C9" s="0">
-        <v>372643.444394992</v>
+        <v>248811.959870538</v>
       </c>
       <c r="D9" s="0">
-        <v>531521.417913735</v>
+        <v>776306.55922755</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>252688.740497776</v>
+        <v>381515.553864425</v>
       </c>
       <c r="B10" s="0">
-        <v>918896.743524306</v>
+        <v>854675.120606401</v>
       </c>
       <c r="C10" s="0">
-        <v>800246.906373765</v>
+        <v>37893.4806389238</v>
       </c>
       <c r="D10" s="0">
-        <v>516078.504508398</v>
+        <v>118266.657515553</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>835999.052895233</v>
+        <v>212359.353533182</v>
       </c>
       <c r="B11" s="0">
-        <v>177828.063805508</v>
+        <v>305640.788891185</v>
       </c>
       <c r="C11" s="0">
-        <v>657742.028896577</v>
+        <v>422221.615641481</v>
       </c>
       <c r="D11" s="0">
-        <v>717118.58441919</v>
+        <v>317343.752047673</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>980791.767584529</v>
+        <v>4954.98022295301</v>
       </c>
       <c r="B12" s="0">
-        <v>631979.440167537</v>
+        <v>89636.4693015984</v>
       </c>
       <c r="C12" s="0">
-        <v>861271.728696894</v>
+        <v>527091.524809176</v>
       </c>
       <c r="D12" s="0">
-        <v>548780.173784485</v>
+        <v>366458.584259478</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>475757.466385028</v>
+        <v>75464.0628935136</v>
       </c>
       <c r="B13" s="0">
-        <v>188960.265456215</v>
+        <v>270947.822495805</v>
       </c>
       <c r="C13" s="0">
-        <v>469860.295983898</v>
+        <v>307977.762682353</v>
       </c>
       <c r="D13" s="0">
-        <v>43082.1180544245</v>
+        <v>229053.272972374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>701464.541117411</v>
+        <v>377902.381298087</v>
       </c>
       <c r="B14" s="0">
-        <v>187941.053038436</v>
+        <v>951168.202306688</v>
       </c>
       <c r="C14" s="0">
-        <v>7382.65412272078</v>
+        <v>506349.161968729</v>
       </c>
       <c r="D14" s="0">
-        <v>940691.097146222</v>
+        <v>947224.474953126</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>828933.774413976</v>
+        <v>161267.614532852</v>
       </c>
       <c r="B15" s="0">
-        <v>617759.728160575</v>
+        <v>603853.411788053</v>
       </c>
       <c r="C15" s="0">
-        <v>659837.366389035</v>
+        <v>203258.294706819</v>
       </c>
       <c r="D15" s="0">
-        <v>756674.185747595</v>
+        <v>770962.758814433</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>180453.655859667</v>
+        <v>961597.156227379</v>
       </c>
       <c r="B16" s="0">
-        <v>192655.787892945</v>
+        <v>210381.322638309</v>
       </c>
       <c r="C16" s="0">
-        <v>368151.575964015</v>
+        <v>266890.916166311</v>
       </c>
       <c r="D16" s="0">
-        <v>49550.5160882839</v>
+        <v>313120.683800951</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>575930.32511693</v>
+        <v>881755.295154525</v>
       </c>
       <c r="B17" s="0">
-        <v>473409.526736201</v>
+        <v>398564.913030046</v>
       </c>
       <c r="C17" s="0">
-        <v>399058.053455808</v>
+        <v>861905.271588781</v>
       </c>
       <c r="D17" s="0">
-        <v>53518.2748239107</v>
+        <v>246628.507155286</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>738896.976103493</v>
+        <v>157552.247009032</v>
       </c>
       <c r="B18" s="0">
-        <v>789012.857148896</v>
+        <v>484340.642804439</v>
       </c>
       <c r="C18" s="0">
-        <v>321516.603846809</v>
+        <v>944072.185523842</v>
       </c>
       <c r="D18" s="0">
-        <v>719709.594603493</v>
+        <v>617452.754926613</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>312554.611504336</v>
+        <v>656692.083765144</v>
       </c>
       <c r="B19" s="0">
-        <v>815007.853701249</v>
+        <v>736505.239613589</v>
       </c>
       <c r="C19" s="0">
-        <v>804272.692093753</v>
+        <v>855346.16227045</v>
       </c>
       <c r="D19" s="0">
-        <v>631303.336765293</v>
+        <v>672500.01042732</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>389871.550439797</v>
+        <v>841504.356750056</v>
       </c>
       <c r="B20" s="0">
-        <v>781342.201298728</v>
+        <v>450736.408797436</v>
       </c>
       <c r="C20" s="0">
-        <v>329561.326340568</v>
+        <v>19758.6868981638</v>
       </c>
       <c r="D20" s="0">
-        <v>4965.96051611284</v>
+        <v>679318.482838254</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>64747.6874593402</v>
+        <v>430347.351557737</v>
       </c>
       <c r="B21" s="0">
-        <v>911514.089401585</v>
+        <v>348325.958637672</v>
       </c>
       <c r="C21" s="0">
-        <v>859555.809227543</v>
+        <v>90669.0056857974</v>
       </c>
       <c r="D21" s="0">
-        <v>512603.274319602</v>
+        <v>755420.004835082</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>218239.324734658</v>
+        <v>608505.941745129</v>
       </c>
       <c r="B22" s="0">
-        <v>517990.697416473</v>
+        <v>102382.494184367</v>
       </c>
       <c r="C22" s="0">
-        <v>901067.843148982</v>
+        <v>651258.856827048</v>
       </c>
       <c r="D22" s="0">
-        <v>256163.180925028</v>
+        <v>322174.468227743</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>788135.979691584</v>
+        <v>794573.657584644</v>
       </c>
       <c r="B23" s="0">
-        <v>263827.864203522</v>
+        <v>822745.553135288</v>
       </c>
       <c r="C23" s="0">
-        <v>811721.21260861</v>
+        <v>213970.841008225</v>
       </c>
       <c r="D23" s="0">
-        <v>606241.77549325</v>
+        <v>590879.810783491</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>2347.93964882751</v>
+        <v>676899.149863468</v>
       </c>
       <c r="B24" s="0">
-        <v>789902.212000406</v>
+        <v>409042.550907024</v>
       </c>
       <c r="C24" s="0">
-        <v>416342.021159987</v>
+        <v>61349.2555270667</v>
       </c>
       <c r="D24" s="0">
-        <v>399045.023787322</v>
+        <v>977827.960614966</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>912451.683968516</v>
+        <v>893561.738493648</v>
       </c>
       <c r="B25" s="0">
-        <v>866424.449191626</v>
+        <v>7096.01678284631</v>
       </c>
       <c r="C25" s="0">
-        <v>287673.059519228</v>
+        <v>888896.407042116</v>
       </c>
       <c r="D25" s="0">
-        <v>467788.052031672</v>
+        <v>17895.9230044372</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>13925.9207127271</v>
+        <v>424762.374919263</v>
       </c>
       <c r="B26" s="0">
-        <v>813487.036066822</v>
+        <v>748507.249517603</v>
       </c>
       <c r="C26" s="0">
-        <v>28534.0296237422</v>
+        <v>530758.284279499</v>
       </c>
       <c r="D26" s="0">
-        <v>578461.796314671</v>
+        <v>702295.217990081</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>399111.454560939</v>
+        <v>510860.747429943</v>
       </c>
       <c r="B27" s="0">
-        <v>863094.461552377</v>
+        <v>190622.635740145</v>
       </c>
       <c r="C27" s="0">
-        <v>363185.615447902</v>
+        <v>587572.433328057</v>
       </c>
       <c r="D27" s="0">
-        <v>476738.436369569</v>
+        <v>820613.94388816</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>664416.235715345</v>
+        <v>533429.336516852</v>
       </c>
       <c r="B28" s="0">
-        <v>613853.717508658</v>
+        <v>307895.907344248</v>
       </c>
       <c r="C28" s="0">
-        <v>886454.779136206</v>
+        <v>106485.266753698</v>
       </c>
       <c r="D28" s="0">
-        <v>7257.07458670115</v>
+        <v>217021.279603718</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>220906.27868702</v>
+        <v>55169.7528246649</v>
       </c>
       <c r="B29" s="0">
-        <v>887945.013999913</v>
+        <v>833081.78597739</v>
       </c>
       <c r="C29" s="0">
-        <v>65353.4229217812</v>
+        <v>621897.717296098</v>
       </c>
       <c r="D29" s="0">
-        <v>331678.724070861</v>
+        <v>596018.029188746</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>48726.7473008143</v>
+        <v>833946.530629856</v>
       </c>
       <c r="B30" s="0">
-        <v>3286.64109263878</v>
+        <v>522534.398605365</v>
       </c>
       <c r="C30" s="0">
-        <v>198030.916600503</v>
+        <v>264466.35148696</v>
       </c>
       <c r="D30" s="0">
-        <v>427570.612368905</v>
+        <v>54578.0542560751</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>599969.338439391</v>
+        <v>432461.805843032</v>
       </c>
       <c r="B31" s="0">
-        <v>365000.180138741</v>
+        <v>389387.153270369</v>
       </c>
       <c r="C31" s="0">
-        <v>930516.302553246</v>
+        <v>41930.7262831976</v>
       </c>
       <c r="D31" s="0">
-        <v>217307.479221983</v>
+        <v>739882.653457989</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>198323.238267714</v>
+        <v>423251.334774891</v>
       </c>
       <c r="B32" s="0">
-        <v>623841.029882357</v>
+        <v>459429.551595556</v>
       </c>
       <c r="C32" s="0">
-        <v>391767.757195871</v>
+        <v>72773.0826813602</v>
       </c>
       <c r="D32" s="0">
-        <v>821682.655635142</v>
+        <v>49265.4359197549</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>404752.288667835</v>
+        <v>859998.692227527</v>
       </c>
       <c r="B33" s="0">
-        <v>489456.66779273</v>
+        <v>571624.209904868</v>
       </c>
       <c r="C33" s="0">
-        <v>322606.046834312</v>
+        <v>948963.638836967</v>
       </c>
       <c r="D33" s="0">
-        <v>185079.327870663</v>
+        <v>168509.54115787</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>925041.518139207</v>
+        <v>603951.021844498</v>
       </c>
       <c r="B34" s="0">
-        <v>900642.24875562</v>
+        <v>235173.119807231</v>
       </c>
       <c r="C34" s="0">
-        <v>334982.776239041</v>
+        <v>393356.897120065</v>
       </c>
       <c r="D34" s="0">
-        <v>728451.064661355</v>
+        <v>245648.38886524</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>388494.22214017</v>
+        <v>369003.24251922</v>
       </c>
       <c r="B35" s="0">
-        <v>903447.4328642</v>
+        <v>302557.284153326</v>
       </c>
       <c r="C35" s="0">
-        <v>409084.946573286</v>
+        <v>844327.975923348</v>
       </c>
       <c r="D35" s="0">
-        <v>973247.254254877</v>
+        <v>335108.590002688</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>24506.6699686026</v>
+        <v>60479.9525162577</v>
       </c>
       <c r="B36" s="0">
-        <v>801071.026269845</v>
+        <v>385198.299486748</v>
       </c>
       <c r="C36" s="0">
-        <v>955994.335448367</v>
+        <v>292878.37785337</v>
       </c>
       <c r="D36" s="0">
-        <v>783020.986608705</v>
+        <v>883141.028640392</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>10639.2796200883</v>
+        <v>902227.976313898</v>
       </c>
       <c r="B37" s="0">
-        <v>615456.11946632</v>
+        <v>484040.898030643</v>
       </c>
       <c r="C37" s="0">
-        <v>600963.417254837</v>
+        <v>476180.230023423</v>
       </c>
       <c r="D37" s="0">
-        <v>402597.346530574</v>
+        <v>310526.827029198</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>34111.2744221982</v>
+        <v>121473.594159574</v>
       </c>
       <c r="B38" s="0">
-        <v>932578.158999131</v>
+        <v>148691.909456948</v>
       </c>
       <c r="C38" s="0">
-        <v>145878.136225919</v>
+        <v>847689.779870068</v>
       </c>
       <c r="D38" s="0">
-        <v>816378.040619371</v>
+        <v>221668.942469018</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>40575.2058329877</v>
+        <v>73999.7849212958</v>
       </c>
       <c r="B39" s="0">
-        <v>222085.960312786</v>
+        <v>235122.824662888</v>
       </c>
       <c r="C39" s="0">
-        <v>64772.1235010643</v>
+        <v>57219.8308339435</v>
       </c>
       <c r="D39" s="0">
-        <v>974921.795062219</v>
+        <v>612176.426971413</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>731449.61089429</v>
+        <v>483545.542919797</v>
       </c>
       <c r="B40" s="0">
-        <v>565338.967165602</v>
+        <v>884118.147140424</v>
       </c>
       <c r="C40" s="0">
-        <v>880274.095051118</v>
+        <v>453388.176138228</v>
       </c>
       <c r="D40" s="0">
-        <v>342759.308099169</v>
+        <v>85444.0508808215</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>148084.498545194</v>
+        <v>598773.410822625</v>
       </c>
       <c r="B41" s="0">
-        <v>668303.864853598</v>
+        <v>129177.5014853</v>
       </c>
       <c r="C41" s="0">
-        <v>469579.851939147</v>
+        <v>18817.9626217196</v>
       </c>
       <c r="D41" s="0">
-        <v>888254.123687863</v>
+        <v>970085.434601682</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>696521.905575191</v>
+        <v>129904.521689706</v>
       </c>
       <c r="B42" s="0">
-        <v>955915.233565455</v>
+        <v>545059.177347021</v>
       </c>
       <c r="C42" s="0">
-        <v>957269.048298369</v>
+        <v>706822.13628051</v>
       </c>
       <c r="D42" s="0">
-        <v>650555.276614872</v>
+        <v>855616.57690239</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>397252.211997869</v>
+        <v>38053.0352881425</v>
       </c>
       <c r="B43" s="0">
-        <v>667846.69443399</v>
+        <v>166551.173742186</v>
       </c>
       <c r="C43" s="0">
-        <v>608746.770587166</v>
+        <v>189632.054040968</v>
       </c>
       <c r="D43" s="0">
-        <v>179488.784251497</v>
+        <v>177057.397634283</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>789296.169201516</v>
+        <v>375957.794196884</v>
       </c>
       <c r="B44" s="0">
-        <v>888493.250537893</v>
+        <v>95443.9798814449</v>
       </c>
       <c r="C44" s="0">
-        <v>920008.700303737</v>
+        <v>638436.811807769</v>
       </c>
       <c r="D44" s="0">
-        <v>713964.813255689</v>
+        <v>447306.419931029</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>992463.359140075</v>
+        <v>455259.112387551</v>
       </c>
       <c r="B45" s="0">
-        <v>754764.112529701</v>
+        <v>387483.339937163</v>
       </c>
       <c r="C45" s="0">
-        <v>518604.73561967</v>
+        <v>171687.954651047</v>
       </c>
       <c r="D45" s="0">
-        <v>48983.5920971742</v>
+        <v>323668.30172188</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>166408.261827383</v>
+        <v>133880.417856332</v>
       </c>
       <c r="B46" s="0">
-        <v>838675.309363136</v>
+        <v>245337.453319383</v>
       </c>
       <c r="C46" s="0">
-        <v>434163.151511067</v>
+        <v>232151.548951935</v>
       </c>
       <c r="D46" s="0">
-        <v>952201.773390268</v>
+        <v>552387.911617937</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>459167.702803001</v>
+        <v>176361.805375834</v>
       </c>
       <c r="B47" s="0">
-        <v>920796.931218727</v>
+        <v>931810.12334852</v>
       </c>
       <c r="C47" s="0">
-        <v>613235.027349198</v>
+        <v>207434.326972549</v>
       </c>
       <c r="D47" s="0">
-        <v>23295.4393249449</v>
+        <v>352337.156120845</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>342335.41476649</v>
+        <v>773050.474828598</v>
       </c>
       <c r="B48" s="0">
-        <v>145876.267527172</v>
+        <v>465222.935408923</v>
       </c>
       <c r="C48" s="0">
-        <v>712709.293566974</v>
+        <v>506094.795421741</v>
       </c>
       <c r="D48" s="0">
-        <v>615227.118886647</v>
+        <v>287761.678587534</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>78196.0408567433</v>
+        <v>576414.416812553</v>
       </c>
       <c r="B49" s="0">
-        <v>975309.110700762</v>
+        <v>441869.773176438</v>
       </c>
       <c r="C49" s="0">
-        <v>495322.859611047</v>
+        <v>992073.202967678</v>
       </c>
       <c r="D49" s="0">
-        <v>180524.314837774</v>
+        <v>683203.893566133</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>372728.511398997</v>
+        <v>907448.61117911</v>
       </c>
       <c r="B50" s="0">
-        <v>613339.18972562</v>
+        <v>45490.7706219194</v>
       </c>
       <c r="C50" s="0">
-        <v>885283.339249568</v>
+        <v>880162.43319966</v>
       </c>
       <c r="D50" s="0">
-        <v>953225.795157825</v>
+        <v>909559.550653007</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>842956.360356396</v>
+        <v>388101.563038352</v>
       </c>
       <c r="B51" s="0">
-        <v>645330.266861864</v>
+        <v>245681.335332655</v>
       </c>
       <c r="C51" s="0">
-        <v>166309.28179543</v>
+        <v>6081.75620719872</v>
       </c>
       <c r="D51" s="0">
-        <v>387951.166549675</v>
+        <v>696343.666732471</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>393320.386015494</v>
+        <v>211290.070885462</v>
       </c>
       <c r="B52" s="0">
-        <v>149699.129233928</v>
+        <v>957489.546834253</v>
       </c>
       <c r="C52" s="0">
-        <v>420596.259841973</v>
+        <v>695149.660899839</v>
       </c>
       <c r="D52" s="0">
-        <v>389512.840839807</v>
+        <v>959592.599868585</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>857846.596212055</v>
+        <v>884567.068370323</v>
       </c>
       <c r="B53" s="0">
-        <v>521752.082054388</v>
+        <v>312907.628395086</v>
       </c>
       <c r="C53" s="0">
-        <v>5067.27490810085</v>
+        <v>154434.224662573</v>
       </c>
       <c r="D53" s="0">
-        <v>815252.684902052</v>
+        <v>454896.043266587</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>476455.280779142</v>
+        <v>106242.911939622</v>
       </c>
       <c r="B54" s="0">
-        <v>54611.6670847925</v>
+        <v>959116.846769637</v>
       </c>
       <c r="C54" s="0">
-        <v>585451.331262221</v>
+        <v>837294.897920124</v>
       </c>
       <c r="D54" s="0">
-        <v>685379.411413045</v>
+        <v>903622.770171437</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>643419.901674343</v>
+        <v>910734.858787961</v>
       </c>
       <c r="B55" s="0">
-        <v>175783.956970919</v>
+        <v>589349.184459704</v>
       </c>
       <c r="C55" s="0">
-        <v>304781.58141709</v>
+        <v>350675.133220234</v>
       </c>
       <c r="D55" s="0">
-        <v>939372.204215905</v>
+        <v>856007.820393894</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>17154.248439313</v>
+        <v>13389.3392111125</v>
       </c>
       <c r="B56" s="0">
-        <v>259441.252918654</v>
+        <v>395410.136969485</v>
       </c>
       <c r="C56" s="0">
-        <v>338080.420781896</v>
+        <v>488484.061084913</v>
       </c>
       <c r="D56" s="0">
-        <v>766768.331530862</v>
+        <v>439741.249866663</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>553069.072101763</v>
+        <v>88389.6472344127</v>
       </c>
       <c r="B57" s="0">
-        <v>953391.970113568</v>
+        <v>365175.020119722</v>
       </c>
       <c r="C57" s="0">
-        <v>480937.356353243</v>
+        <v>322591.998298928</v>
       </c>
       <c r="D57" s="0">
-        <v>720452.461727174</v>
+        <v>145625.027430069</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>813837.435941136</v>
+        <v>930680.470043179</v>
       </c>
       <c r="B58" s="0">
-        <v>754487.649423297</v>
+        <v>925728.367141321</v>
       </c>
       <c r="C58" s="0">
-        <v>225283.860799523</v>
+        <v>511090.660240078</v>
       </c>
       <c r="D58" s="0">
-        <v>256033.25118126</v>
+        <v>276792.395988848</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>192636.285532562</v>
+        <v>815560.927994345</v>
       </c>
       <c r="B59" s="0">
-        <v>725280.007685199</v>
+        <v>770073.274509084</v>
       </c>
       <c r="C59" s="0">
-        <v>323196.452727167</v>
+        <v>546502.195553157</v>
       </c>
       <c r="D59" s="0">
-        <v>994265.153070104</v>
+        <v>398876.948002203</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>556443.958802355</v>
+        <v>263506.788417467</v>
       </c>
       <c r="B60" s="0">
-        <v>970241.835792662</v>
+        <v>287435.548513865</v>
       </c>
       <c r="C60" s="0">
-        <v>680070.174708995</v>
+        <v>537177.159701091</v>
       </c>
       <c r="D60" s="0">
-        <v>3838.29185917894</v>
+        <v>321100.650039083</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>318116.844314205</v>
+        <v>948331.764409473</v>
       </c>
       <c r="B61" s="0">
-        <v>27887.858463399</v>
+        <v>208195.872701796</v>
       </c>
       <c r="C61" s="0">
-        <v>199903.927836522</v>
+        <v>976539.663028223</v>
       </c>
       <c r="D61" s="0">
-        <v>273865.210019921</v>
+        <v>979993.149163198</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>667172.403385477</v>
+        <v>798752.378578648</v>
       </c>
       <c r="B62" s="0">
-        <v>340548.685444774</v>
+        <v>895006.202112421</v>
       </c>
       <c r="C62" s="0">
-        <v>226937.077579525</v>
+        <v>150073.935813305</v>
       </c>
       <c r="D62" s="0">
-        <v>511339.065856924</v>
+        <v>883657.699396674</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>133879.13309684</v>
+        <v>815879.933915976</v>
       </c>
       <c r="B63" s="0">
-        <v>811618.708452032</v>
+        <v>469005.48574934</v>
       </c>
       <c r="C63" s="0">
-        <v>653827.928311111</v>
+        <v>255408.411033176</v>
       </c>
       <c r="D63" s="0">
-        <v>263500.06939075</v>
+        <v>856548.376314597</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>904454.626098487</v>
+        <v>519392.048250601</v>
       </c>
       <c r="B64" s="0">
-        <v>40814.7257011452</v>
+        <v>990315.630096158</v>
       </c>
       <c r="C64" s="0">
-        <v>284614.813180927</v>
+        <v>8809.197232504</v>
       </c>
       <c r="D64" s="0">
-        <v>822906.453545627</v>
+        <v>442277.072669136</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>721967.631355844</v>
+        <v>180514.544798301</v>
       </c>
       <c r="B65" s="0">
-        <v>829327.806285269</v>
+        <v>448026.186529559</v>
       </c>
       <c r="C65" s="0">
-        <v>329418.080080961</v>
+        <v>560502.501931275</v>
       </c>
       <c r="D65" s="0">
-        <v>584590.424590088</v>
+        <v>841478.213594052</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>918139.893989144</v>
+        <v>140661.584278877</v>
       </c>
       <c r="B66" s="0">
-        <v>852587.504243752</v>
+        <v>42846.988906547</v>
       </c>
       <c r="C66" s="0">
-        <v>310516.428346986</v>
+        <v>951798.185218032</v>
       </c>
       <c r="D66" s="0">
-        <v>22626.1913881759</v>
+        <v>149276.289227082</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>46912.4126466515</v>
+        <v>725953.790697248</v>
       </c>
       <c r="B67" s="0">
-        <v>579371.078209659</v>
+        <v>858232.977268395</v>
       </c>
       <c r="C67" s="0">
-        <v>334242.128922717</v>
+        <v>167383.41104583</v>
       </c>
       <c r="D67" s="0">
-        <v>961008.351743691</v>
+        <v>662057.109951068</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>525181.213638364</v>
+        <v>880193.774532617</v>
       </c>
       <c r="B68" s="0">
-        <v>753488.042277046</v>
+        <v>388635.357091499</v>
       </c>
       <c r="C68" s="0">
-        <v>207072.146333322</v>
+        <v>342598.84913573</v>
       </c>
       <c r="D68" s="0">
-        <v>132123.051738424</v>
+        <v>649597.002030163</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>473288.750496362</v>
+        <v>35674.2679307583</v>
       </c>
       <c r="B69" s="0">
-        <v>527550.571843772</v>
+        <v>775654.431328016</v>
       </c>
       <c r="C69" s="0">
-        <v>713944.794942599</v>
+        <v>627432.960843403</v>
       </c>
       <c r="D69" s="0">
-        <v>505925.311476889</v>
+        <v>214636.975067964</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>381017.57708053</v>
+        <v>346555.442245004</v>
       </c>
       <c r="B70" s="0">
-        <v>71452.079374088</v>
+        <v>514664.863475908</v>
       </c>
       <c r="C70" s="0">
-        <v>59696.3833364176</v>
+        <v>689953.819238559</v>
       </c>
       <c r="D70" s="0">
-        <v>926372.259355324</v>
+        <v>598381.864651284</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>515629.23310121</v>
+        <v>273191.158321309</v>
       </c>
       <c r="B71" s="0">
-        <v>685627.022611735</v>
+        <v>278626.351281361</v>
       </c>
       <c r="C71" s="0">
-        <v>857163.721163368</v>
+        <v>94900.0870319549</v>
       </c>
       <c r="D71" s="0">
-        <v>640989.70482172</v>
+        <v>889677.876555211</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>488789.038028935</v>
+        <v>500305.577879914</v>
       </c>
       <c r="B72" s="0">
-        <v>698469.778382438</v>
+        <v>647693.37077052</v>
       </c>
       <c r="C72" s="0">
-        <v>615313.503246435</v>
+        <v>135061.449434171</v>
       </c>
       <c r="D72" s="0">
-        <v>787140.910414579</v>
+        <v>865987.675667735</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>814584.899141726</v>
+        <v>755905.389672101</v>
       </c>
       <c r="B73" s="0">
-        <v>30032.2570977883</v>
+        <v>943208.016894389</v>
       </c>
       <c r="C73" s="0">
-        <v>204310.886191349</v>
+        <v>797.646586223341</v>
       </c>
       <c r="D73" s="0">
-        <v>191170.923966528</v>
+        <v>334478.520478345</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>554508.054887181</v>
+        <v>957646.956647582</v>
       </c>
       <c r="B74" s="0">
-        <v>477376.579529316</v>
+        <v>301622.07470351</v>
       </c>
       <c r="C74" s="0">
-        <v>692819.576567421</v>
+        <v>593351.301082108</v>
       </c>
       <c r="D74" s="0">
-        <v>455604.142255897</v>
+        <v>701835.917170083</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>150966.583821441</v>
+        <v>130756.691159102</v>
       </c>
       <c r="B75" s="0">
-        <v>833742.579367823</v>
+        <v>647716.780960428</v>
       </c>
       <c r="C75" s="0">
-        <v>152491.761442503</v>
+        <v>359212.195202341</v>
       </c>
       <c r="D75" s="0">
-        <v>497732.62557468</v>
+        <v>228410.480650333</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>194417.059512072</v>
+        <v>404860.113470284</v>
       </c>
       <c r="B76" s="0">
-        <v>115383.01134267</v>
+        <v>820593.225686156</v>
       </c>
       <c r="C76" s="0">
-        <v>823492.768604072</v>
+        <v>345865.526863311</v>
       </c>
       <c r="D76" s="0">
-        <v>617680.57086397</v>
+        <v>595213.590932644</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>846687.814615056</v>
+        <v>625996.720802969</v>
       </c>
       <c r="B77" s="0">
-        <v>792891.120907334</v>
+        <v>352893.169667988</v>
       </c>
       <c r="C77" s="0">
-        <v>384144.168991663</v>
+        <v>353416.320566748</v>
       </c>
       <c r="D77" s="0">
-        <v>10334.8046589339</v>
+        <v>961936.80631087</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>361285.390034917</v>
+        <v>447327.439415887</v>
       </c>
       <c r="B78" s="0">
-        <v>722207.357046291</v>
+        <v>763332.89023644</v>
       </c>
       <c r="C78" s="0">
-        <v>693252.424100997</v>
+        <v>277705.53449062</v>
       </c>
       <c r="D78" s="0">
-        <v>877216.003312364</v>
+        <v>64887.5148337742</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>826711.435255926</v>
+        <v>232500.403762097</v>
       </c>
       <c r="B79" s="0">
-        <v>138174.539030611</v>
+        <v>253573.907657328</v>
       </c>
       <c r="C79" s="0">
-        <v>419931.235918743</v>
+        <v>476611.173467995</v>
       </c>
       <c r="D79" s="0">
-        <v>461933.535738817</v>
+        <v>294230.560909133</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>443256.493398573</v>
+        <v>92466.2510363694</v>
       </c>
       <c r="B80" s="0">
-        <v>323239.685652423</v>
+        <v>774856.784741793</v>
       </c>
       <c r="C80" s="0">
-        <v>522773.870976071</v>
+        <v>292954.440365059</v>
       </c>
       <c r="D80" s="0">
-        <v>802729.784419169</v>
+        <v>878435.344844328</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>903640.997551214</v>
+        <v>44933.3675414945</v>
       </c>
       <c r="B81" s="0">
-        <v>378632.502806667</v>
+        <v>921313.5623938</v>
       </c>
       <c r="C81" s="0">
-        <v>604092.241080521</v>
+        <v>988117.902068476</v>
       </c>
       <c r="D81" s="0">
-        <v>383660.579278907</v>
+        <v>678080.555832982</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>681886.653733387</v>
+        <v>625474.377360882</v>
       </c>
       <c r="B82" s="0">
-        <v>533135.261169232</v>
+        <v>919414.156079019</v>
       </c>
       <c r="C82" s="0">
-        <v>359431.095588687</v>
+        <v>866489.606381622</v>
       </c>
       <c r="D82" s="0">
-        <v>751429.868280622</v>
+        <v>493929.371002097</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>373406.026686265</v>
+        <v>679712.352193758</v>
       </c>
       <c r="B83" s="0">
-        <v>874977.009778366</v>
+        <v>301827.843907209</v>
       </c>
       <c r="C83" s="0">
-        <v>997632.932382465</v>
+        <v>539847.858501527</v>
       </c>
       <c r="D83" s="0">
-        <v>681434.187889767</v>
+        <v>98537.6444172755</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>21693.7782343914</v>
+        <v>403012.220004114</v>
       </c>
       <c r="B84" s="0">
-        <v>645888.088106126</v>
+        <v>589791.696327641</v>
       </c>
       <c r="C84" s="0">
-        <v>193976.081532415</v>
+        <v>38860.8402753532</v>
       </c>
       <c r="D84" s="0">
-        <v>386632.015177343</v>
+        <v>58490.4998813246</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>832300.69784089</v>
+        <v>194314.066411142</v>
       </c>
       <c r="B85" s="0">
-        <v>784124.155428318</v>
+        <v>23916.5402128904</v>
       </c>
       <c r="C85" s="0">
-        <v>815603.573255056</v>
+        <v>528463.786248334</v>
       </c>
       <c r="D85" s="0">
-        <v>136497.253149979</v>
+        <v>47429.0359054827</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>12792.0447908305</v>
+        <v>877182.783501773</v>
       </c>
       <c r="B86" s="0">
-        <v>413811.34344908</v>
+        <v>171105.607492433</v>
       </c>
       <c r="C86" s="0">
-        <v>690558.225703686</v>
+        <v>64981.6342932087</v>
       </c>
       <c r="D86" s="0">
-        <v>987143.696745459</v>
+        <v>770449.278303631</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>871177.373859648</v>
+        <v>630003.328728491</v>
       </c>
       <c r="B87" s="0">
-        <v>592609.1403666</v>
+        <v>527638.785321097</v>
       </c>
       <c r="C87" s="0">
-        <v>20762.9841849036</v>
+        <v>467430.182018983</v>
       </c>
       <c r="D87" s="0">
-        <v>205278.772025033</v>
+        <v>306595.924918817</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>468055.311808388</v>
+        <v>704683.158409168</v>
       </c>
       <c r="B88" s="0">
-        <v>188798.879826813</v>
+        <v>364775.267599512</v>
       </c>
       <c r="C88" s="0">
-        <v>483.589712755564</v>
+        <v>675335.764733765</v>
       </c>
       <c r="D88" s="0">
-        <v>149010.001751133</v>
+        <v>905354.01455376</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>828150.128865684</v>
+        <v>527913.283336867</v>
       </c>
       <c r="B89" s="0">
-        <v>362776.261457604</v>
+        <v>896843.283854818</v>
       </c>
       <c r="C89" s="0">
-        <v>941822.555820375</v>
+        <v>783776.163488522</v>
       </c>
       <c r="D89" s="0">
-        <v>987840.714393109</v>
+        <v>872578.033186765</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>951734.42547756</v>
+        <v>930672.559854888</v>
       </c>
       <c r="B90" s="0">
-        <v>140541.606648146</v>
+        <v>713726.049155801</v>
       </c>
       <c r="C90" s="0">
-        <v>738497.048028976</v>
+        <v>378073.52905072</v>
       </c>
       <c r="D90" s="0">
-        <v>638431.834354266</v>
+        <v>564860.840591072</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>797368.405292448</v>
+        <v>502674.554708728</v>
       </c>
       <c r="B91" s="0">
-        <v>129263.604120008</v>
+        <v>735995.94446644</v>
       </c>
       <c r="C91" s="0">
-        <v>136141.855798728</v>
+        <v>234463.940483734</v>
       </c>
       <c r="D91" s="0">
-        <v>460819.647396365</v>
+        <v>989561.154036578</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>119516.842122896</v>
+        <v>21016.8273286041</v>
       </c>
       <c r="B92" s="0">
-        <v>563028.929551611</v>
+        <v>392849.776145466</v>
       </c>
       <c r="C92" s="0">
-        <v>467594.987930541</v>
+        <v>940688.866162993</v>
       </c>
       <c r="D92" s="0">
-        <v>667660.334458416</v>
+        <v>990279.650776777</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>268075.310284307</v>
+        <v>454368.769868449</v>
       </c>
       <c r="B93" s="0">
-        <v>842577.035465546</v>
+        <v>854432.521785811</v>
       </c>
       <c r="C93" s="0">
-        <v>372287.398843229</v>
+        <v>96040.3280779907</v>
       </c>
       <c r="D93" s="0">
-        <v>305126.525138098</v>
+        <v>190647.116485353</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>780796.886319666</v>
+        <v>152073.566872661</v>
       </c>
       <c r="B94" s="0">
-        <v>854214.025593462</v>
+        <v>834397.661888226</v>
       </c>
       <c r="C94" s="0">
-        <v>792354.160357432</v>
+        <v>233251.93358271</v>
       </c>
       <c r="D94" s="0">
-        <v>479368.46291617</v>
+        <v>376020.980708311</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>832894.898407578</v>
+        <v>38236.9524046019</v>
       </c>
       <c r="B95" s="0">
-        <v>645404.49839337</v>
+        <v>914455.931593876</v>
       </c>
       <c r="C95" s="0">
-        <v>44966.0797812818</v>
+        <v>133506.825721593</v>
       </c>
       <c r="D95" s="0">
-        <v>263979.760121545</v>
+        <v>407976.856645186</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>469524.436383287</v>
+        <v>297470.782556325</v>
       </c>
       <c r="B96" s="0">
-        <v>842301.599607943</v>
+        <v>240140.376724368</v>
       </c>
       <c r="C96" s="0">
-        <v>827762.858861947</v>
+        <v>655885.753061569</v>
       </c>
       <c r="D96" s="0">
-        <v>190796.390730327</v>
+        <v>72734.5068346404</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>872250.438142685</v>
+        <v>163456.734345973</v>
       </c>
       <c r="B97" s="0">
-        <v>675314.295420104</v>
+        <v>793032.078441713</v>
       </c>
       <c r="C97" s="0">
-        <v>52126.3913494192</v>
+        <v>500120.793702137</v>
       </c>
       <c r="D97" s="0">
-        <v>498248.546150629</v>
+        <v>715500.295961043</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>741913.76973964</v>
+        <v>894007.384262051</v>
       </c>
       <c r="B98" s="0">
-        <v>456467.284567872</v>
+        <v>293174.844837363</v>
       </c>
       <c r="C98" s="0">
-        <v>559943.336788539</v>
+        <v>477869.027982405</v>
       </c>
       <c r="D98" s="0">
-        <v>625177.671026987</v>
+        <v>212292.325316133</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>905026.382256777</v>
+        <v>311833.382263702</v>
       </c>
       <c r="B99" s="0">
-        <v>721203.891896272</v>
+        <v>424086.401436518</v>
       </c>
       <c r="C99" s="0">
-        <v>332823.255254339</v>
+        <v>685056.113956988</v>
       </c>
       <c r="D99" s="0">
-        <v>300477.243634163</v>
+        <v>725954.006298424</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>985573.093400138</v>
+        <v>673480.761551056</v>
       </c>
       <c r="B100" s="0">
-        <v>990488.862614375</v>
+        <v>800802.955776827</v>
       </c>
       <c r="C100" s="0">
-        <v>636696.030682277</v>
+        <v>593129.047003169</v>
       </c>
       <c r="D100" s="0">
-        <v>969642.799333503</v>
+        <v>310271.880268246</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>97520.3998840975</v>
+        <v>96274.8979666619</v>
       </c>
       <c r="B101" s="0">
-        <v>348187.446290714</v>
+        <v>480474.115573091</v>
       </c>
       <c r="C101" s="0">
-        <v>259128.585112807</v>
+        <v>2052.54834240887</v>
       </c>
       <c r="D101" s="0">
-        <v>282985.444778104</v>
+        <v>540174.278682179</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>151963.906899078</v>
+        <v>588218.623114852</v>
       </c>
       <c r="B102" s="0">
-        <v>84297.5243387267</v>
+        <v>602489.118744847</v>
       </c>
       <c r="C102" s="0">
-        <v>872162.095677183</v>
+        <v>826487.083838548</v>
       </c>
       <c r="D102" s="0">
-        <v>947059.639239246</v>
+        <v>628600.246565696</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>277215.242514953</v>
+        <v>780876.450604236</v>
       </c>
       <c r="B103" s="0">
-        <v>735266.070689664</v>
+        <v>736964.023083897</v>
       </c>
       <c r="C103" s="0">
-        <v>276798.597200214</v>
+        <v>867954.359328353</v>
       </c>
       <c r="D103" s="0">
-        <v>903394.515115486</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="0">
-        <v>592761.014864203</v>
-      </c>
-      <c r="B104" s="0">
-        <v>790450.644116127</v>
-      </c>
-      <c r="C104" s="0">
-        <v>874038.8526926</v>
-      </c>
-      <c r="D104" s="0">
-        <v>656191.587288022</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="0">
-        <v>324329.601751794</v>
-      </c>
-      <c r="B105" s="0">
-        <v>294270.688804924</v>
-      </c>
-      <c r="C105" s="0">
-        <v>167176.489330445</v>
-      </c>
-      <c r="D105" s="0">
-        <v>396819.580065468</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="0">
-        <v>111691.006511306</v>
-      </c>
-      <c r="B106" s="0">
-        <v>312581.243139031</v>
-      </c>
-      <c r="C106" s="0">
-        <v>744488.836147119</v>
-      </c>
-      <c r="D106" s="0">
-        <v>409402.815350053</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="0">
-        <v>479035.573768912</v>
-      </c>
-      <c r="B107" s="0">
-        <v>205605.568925666</v>
-      </c>
-      <c r="C107" s="0">
-        <v>858120.059528444</v>
-      </c>
-      <c r="D107" s="0">
-        <v>25892.4146303406</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="0">
-        <v>524062.99185197</v>
-      </c>
-      <c r="B108" s="0">
-        <v>416185.710307297</v>
-      </c>
-      <c r="C108" s="0">
-        <v>769140.946571315</v>
-      </c>
-      <c r="D108" s="0">
-        <v>842248.293963377</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="0">
-        <v>657616.245400913</v>
-      </c>
-      <c r="B109" s="0">
-        <v>584305.188890689</v>
-      </c>
-      <c r="C109" s="0">
-        <v>612883.697549293</v>
-      </c>
-      <c r="D109" s="0">
-        <v>514601.006412227</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="0">
-        <v>169760.311567113</v>
-      </c>
-      <c r="B110" s="0">
-        <v>444405.294696058</v>
-      </c>
-      <c r="C110" s="0">
-        <v>429428.740138853</v>
-      </c>
-      <c r="D110" s="0">
-        <v>324194.923659877</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="0">
-        <v>195122.449284011</v>
-      </c>
-      <c r="B111" s="0">
-        <v>116450.009921775</v>
-      </c>
-      <c r="C111" s="0">
-        <v>980504.443394255</v>
-      </c>
-      <c r="D111" s="0">
-        <v>693358.654013536</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="0">
-        <v>803249.711079173</v>
-      </c>
-      <c r="B112" s="0">
-        <v>181010.95696027</v>
-      </c>
-      <c r="C112" s="0">
-        <v>862309.005047339</v>
-      </c>
-      <c r="D112" s="0">
-        <v>832565.437458719</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="0">
-        <v>839382.663760047</v>
-      </c>
-      <c r="B113" s="0">
-        <v>339808.688191608</v>
-      </c>
-      <c r="C113" s="0">
-        <v>462759.28032713</v>
-      </c>
-      <c r="D113" s="0">
-        <v>418872.724482265</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="0">
-        <v>71609.6735892862</v>
-      </c>
-      <c r="B114" s="0">
-        <v>877146.01116122</v>
-      </c>
-      <c r="C114" s="0">
-        <v>250906.182569874</v>
-      </c>
-      <c r="D114" s="0">
-        <v>236649.095656653</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="0">
-        <v>176575.304556906</v>
-      </c>
-      <c r="B115" s="0">
-        <v>21309.6975448121</v>
-      </c>
-      <c r="C115" s="0">
-        <v>31790.5587292232</v>
-      </c>
-      <c r="D115" s="0">
-        <v>159220.556337023</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="0">
-        <v>740024.412861105</v>
-      </c>
-      <c r="B116" s="0">
-        <v>681386.991255631</v>
-      </c>
-      <c r="C116" s="0">
-        <v>652575.482918218</v>
-      </c>
-      <c r="D116" s="0">
-        <v>591485.939729719</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="0">
-        <v>667285.711815248</v>
-      </c>
-      <c r="B117" s="0">
-        <v>883152.503000178</v>
-      </c>
-      <c r="C117" s="0">
-        <v>420293.912487241</v>
-      </c>
-      <c r="D117" s="0">
-        <v>147586.885442765</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="0">
-        <v>362585.563847136</v>
-      </c>
-      <c r="B118" s="0">
-        <v>225101.125531411</v>
-      </c>
-      <c r="C118" s="0">
-        <v>164761.405514908</v>
-      </c>
-      <c r="D118" s="0">
-        <v>185318.040282148</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="0">
-        <v>343052.0348917</v>
-      </c>
-      <c r="B119" s="0">
-        <v>553876.705259959</v>
-      </c>
-      <c r="C119" s="0">
-        <v>936575.509112596</v>
-      </c>
-      <c r="D119" s="0">
-        <v>297939.04828743</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="0">
-        <v>317807.557209305</v>
-      </c>
-      <c r="B120" s="0">
-        <v>121545.908563559</v>
-      </c>
-      <c r="C120" s="0">
-        <v>194010.973067028</v>
-      </c>
-      <c r="D120" s="0">
-        <v>883059.915566379</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="0">
-        <v>292614.300405893</v>
-      </c>
-      <c r="B121" s="0">
-        <v>193499.112126184</v>
-      </c>
-      <c r="C121" s="0">
-        <v>192779.644482201</v>
-      </c>
-      <c r="D121" s="0">
-        <v>871975.595537562</v>
+        <v>233151.30557546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>